<commit_message>
Added the missing question - tool3_can and shift the tag name in uk-217 to tool4_can
</commit_message>
<xml_diff>
--- a/uk-2017.xlsx
+++ b/uk-2017.xlsx
@@ -631,7 +631,7 @@
     <t xml:space="preserve">What is your Operating System of choice for use at work?</t>
   </si>
   <si>
-    <t xml:space="preserve">tool3_can</t>
+    <t xml:space="preserve">tool4_can</t>
   </si>
   <si>
     <t xml:space="preserve">What programming languages do you use in developing research software? Please list in order, beginning with most frequently used.</t>
@@ -873,22 +873,22 @@
   </sheetPr>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.49489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="80.9132653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.49489795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.4744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.49489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="89.2091836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3316326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5969387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add question ukrse2 and ukrse3C
</commit_message>
<xml_diff>
--- a/uk-2017.xlsx
+++ b/uk-2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="229">
   <si>
     <t xml:space="preserve">Section</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">edu4</t>
   </si>
   <si>
-    <t xml:space="preserve">Do you hold any professional qualifications? If yes, please enter them separated by commas.</t>
+    <t xml:space="preserve">Do you hold any other professional qualifications? If yes, please enter them separated by commas.</t>
   </si>
   <si>
     <t xml:space="preserve">Purpose? Could be removed – way too many possibilities</t>
@@ -130,9 +130,6 @@
     <t xml:space="preserve">To easily filter out those who do not write software</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">rse3</t>
   </si>
   <si>
@@ -145,16 +142,19 @@
     <t xml:space="preserve">Scale from Mostly myself to Mostly other people. To identify whether they're just using their own code, or writing for other people</t>
   </si>
   <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
     <t xml:space="preserve">time1_can</t>
   </si>
   <si>
-    <t xml:space="preserve">In an average month, how much time do you spend on software development</t>
+    <t xml:space="preserve">In an average month, how much time do you spend on software development (Please rate your answer between 1 to 10. 1 Being none at all and 10 being All your time.)</t>
   </si>
   <si>
     <t xml:space="preserve">LIKERT (TIME) 1-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Interval scale: 1 (Never) -2 -3 – 4 – 5 – 6 -7 – 8 – 9 – 10 (All my time)</t>
+    <t xml:space="preserve">Interval scale: 1 (None at all) -2 – 3 – 4 – 5 – 6 -7 – 8 – 9 – 10 (All my time)</t>
   </si>
   <si>
     <t xml:space="preserve">time2_can</t>
@@ -190,9 +190,6 @@
     <t xml:space="preserve">Do you consider yourself a professional software developer?</t>
   </si>
   <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
     <t xml:space="preserve">currentEmp1</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t xml:space="preserve">What was your previous job?</t>
   </si>
   <si>
-    <t xml:space="preserve">dropdown</t>
-  </si>
-  <si>
     <t xml:space="preserve">prevEmp2</t>
   </si>
   <si>
@@ -430,10 +424,25 @@
     <t xml:space="preserve">Is there a technical hand-over plan for your most important software project?</t>
   </si>
   <si>
+    <t xml:space="preserve">open01_can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you release some of the software projects you’ve worked on, under an open source licence or as free software</t>
+  </si>
+  <si>
     <t xml:space="preserve">open1_can</t>
   </si>
   <si>
-    <t xml:space="preserve">What percentage of the software projects you've worked on are released under an open source license?</t>
+    <t xml:space="preserve">What percentage of the software projects you've worked on are released under an open source license or as free software?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if YES to open01_can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open03_can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you associate a Digital Object Identifier (DOI) to some of the software project you’ve worked on?</t>
   </si>
   <si>
     <t xml:space="preserve">open3_can</t>
@@ -442,6 +451,9 @@
     <t xml:space="preserve">What percentage of the software projects you've worked on have an associated Digital Object Identifier (DOI)?</t>
   </si>
   <si>
+    <t xml:space="preserve">if YES to open03_can</t>
+  </si>
+  <si>
     <t xml:space="preserve">perfCheck1</t>
   </si>
   <si>
@@ -646,27 +658,27 @@
     <t xml:space="preserve">https://www.gov.uk/service-manual/user-centred-design/resources/patterns/gender-and-sex.html</t>
   </si>
   <si>
-    <t xml:space="preserve">DROPDOWN</t>
-  </si>
-  <si>
     <t xml:space="preserve">socio3</t>
   </si>
   <si>
-    <t xml:space="preserve">Please select your ethnicity</t>
+    <t xml:space="preserve">Please select your age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socio5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is your ethnicity group</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.academia.edu/1112558/Comparative_study_on_the_collection_of_data_to_measure_the_extent_and_impact_of_discrimination_within_the_United_States_Canada_Australia_the_United_Kingdom_and_the_Netherlands</t>
   </si>
   <si>
-    <t xml:space="preserve">We need to start investigating ethnicity too</t>
+    <t xml:space="preserve">https://www.ons.gov.uk/ons/guide-method/...set-of...questions/ethnic-group.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">socio4</t>
   </si>
   <si>
-    <t xml:space="preserve">Please select your age</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please select the range of your salary</t>
   </si>
   <si>
@@ -674,6 +686,27 @@
   </si>
   <si>
     <t xml:space="preserve">Are you a member of the UK RSE Association? (Members are people who have signed up to the UK RSE mailing list)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukrse2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How did you build your network within the RSE community? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukrse3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please give us details on how you create your network </t>
+  </si>
+  <si>
+    <t xml:space="preserve">if other to ukrse2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukrse4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do we become an RSE</t>
   </si>
 </sst>
 </file>
@@ -683,7 +716,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -748,6 +781,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -791,7 +831,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -844,6 +884,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -858,9 +906,9 @@
       <font>
         <name val="Arial"/>
         <charset val="1"/>
-        <family val="0"/>
-        <color rgb="FF000000"/>
+        <family val="2"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -871,24 +919,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51:D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="89.2091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3928571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="78.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="12.51"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1092,16 +1140,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
@@ -1110,13 +1158,16 @@
         <v>15</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" s="8" t="s">
         <v>41</v>
       </c>
@@ -1137,6 +1188,9 @@
       <c r="A11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>45</v>
       </c>
@@ -1157,6 +1211,9 @@
       <c r="A12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>47</v>
       </c>
@@ -1177,6 +1234,9 @@
       <c r="A13" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>49</v>
       </c>
@@ -1197,6 +1257,9 @@
       <c r="A14" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>51</v>
       </c>
@@ -1212,6 +1275,9 @@
       <c r="A15" s="4" t="n">
         <v>1</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>54</v>
       </c>
@@ -1228,13 +1294,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -1246,7 +1312,7 @@
         <v>15</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1254,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>13</v>
@@ -1269,16 +1335,16 @@
         <v>10</v>
       </c>
       <c r="G17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="I17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1286,13 +1352,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>27</v>
@@ -1301,7 +1367,7 @@
         <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I18" s="0" t="s">
         <v>15</v>
@@ -1312,13 +1378,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>27</v>
@@ -1327,13 +1393,13 @@
         <v>10</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1341,13 +1407,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>27</v>
@@ -1364,13 +1430,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>27</v>
@@ -1382,7 +1448,7 @@
         <v>15</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1391,10 +1457,10 @@
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>34</v>
@@ -1406,7 +1472,7 @@
         <v>15</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1417,10 +1483,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
@@ -1429,13 +1495,13 @@
         <v>10</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1446,13 +1512,13 @@
         <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>10</v>
@@ -1462,7 +1528,7 @@
         <v>15</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1470,13 +1536,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>13</v>
@@ -1485,13 +1551,13 @@
         <v>10</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1502,10 +1568,10 @@
         <v>10</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>53</v>
@@ -1514,7 +1580,7 @@
         <v>10</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>15</v>
@@ -1525,13 +1591,13 @@
         <v>3</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>13</v>
@@ -1548,13 +1614,13 @@
         <v>3</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>13</v>
@@ -1563,13 +1629,13 @@
         <v>10</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I28" s="0" t="s">
         <v>15</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" s="4" customFormat="true" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1577,36 +1643,37 @@
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>71</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
+      <c r="B32" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C32" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>53</v>
@@ -1615,14 +1682,17 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
+      <c r="B33" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C33" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="G33" s="4"/>
     </row>
@@ -1630,35 +1700,40 @@
       <c r="A34" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C34" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C35" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>53</v>
@@ -1674,12 +1749,14 @@
       <c r="A36" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>34</v>
@@ -1696,10 +1773,10 @@
         <v>4</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>34</v>
@@ -1708,19 +1785,21 @@
         <v>10</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C38" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>34</v>
@@ -1729,21 +1808,24 @@
         <v>10</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C39" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>34</v>
@@ -1752,21 +1834,24 @@
         <v>10</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C40" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>34</v>
@@ -1779,18 +1864,21 @@
       <c r="A41" s="4" t="n">
         <v>4</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C41" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J41" s="4"/>
     </row>
@@ -1798,12 +1886,14 @@
       <c r="A42" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C42" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>13</v>
@@ -1817,12 +1907,14 @@
       <c r="A43" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C43" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>34</v>
@@ -1836,98 +1928,118 @@
       <c r="A44" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C44" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" s="4"/>
+        <v>134</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="12" t="s">
-        <v>138</v>
+      <c r="B45" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B46" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C46" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="E46" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="D47" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="4"/>
-    </row>
-    <row r="47" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4" t="s">
+      <c r="E47" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C48" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="E48" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="0" t="s">
-        <v>142</v>
-      </c>
       <c r="F48" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C49" s="4" t="s">
         <v>147</v>
       </c>
@@ -1935,18 +2047,20 @@
         <v>148</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C50" s="4" t="s">
         <v>149</v>
       </c>
@@ -1954,18 +2068,20 @@
         <v>150</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B51" s="4"/>
+      <c r="B51" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C51" s="4" t="s">
         <v>151</v>
       </c>
@@ -1973,18 +2089,20 @@
         <v>152</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B52" s="4"/>
+      <c r="B52" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C52" s="4" t="s">
         <v>153</v>
       </c>
@@ -1992,18 +2110,20 @@
         <v>154</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C53" s="4" t="s">
         <v>155</v>
       </c>
@@ -2011,7 +2131,7 @@
         <v>156</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>10</v>
@@ -2022,7 +2142,9 @@
       <c r="A54" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C54" s="4" t="s">
         <v>157</v>
       </c>
@@ -2030,18 +2152,20 @@
         <v>158</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B55" s="4"/>
+      <c r="B55" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C55" s="4" t="s">
         <v>159</v>
       </c>
@@ -2049,7 +2173,7 @@
         <v>160</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>10</v>
@@ -2060,7 +2184,9 @@
       <c r="A56" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C56" s="4" t="s">
         <v>161</v>
       </c>
@@ -2068,7 +2194,7 @@
         <v>162</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>10</v>
@@ -2079,7 +2205,9 @@
       <c r="A57" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B57" s="4"/>
+      <c r="B57" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C57" s="4" t="s">
         <v>163</v>
       </c>
@@ -2087,7 +2215,7 @@
         <v>164</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>10</v>
@@ -2098,15 +2226,17 @@
       <c r="A58" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C58" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D58" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="E58" s="0" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>10</v>
@@ -2117,15 +2247,17 @@
       <c r="A59" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B59" s="4"/>
+      <c r="B59" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C59" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="E59" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>165</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>10</v>
@@ -2136,7 +2268,9 @@
       <c r="A60" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B60" s="4"/>
+      <c r="B60" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C60" s="4" t="s">
         <v>170</v>
       </c>
@@ -2144,18 +2278,20 @@
         <v>171</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B61" s="4"/>
+      <c r="B61" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C61" s="4" t="s">
         <v>172</v>
       </c>
@@ -2163,18 +2299,20 @@
         <v>173</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C62" s="4" t="s">
         <v>174</v>
       </c>
@@ -2182,18 +2320,20 @@
         <v>175</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="25.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C63" s="4" t="s">
         <v>176</v>
       </c>
@@ -2201,18 +2341,20 @@
         <v>177</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B64" s="4"/>
+      <c r="B64" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C64" s="4" t="s">
         <v>178</v>
       </c>
@@ -2220,18 +2362,20 @@
         <v>179</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B65" s="4"/>
+      <c r="B65" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C65" s="4" t="s">
         <v>180</v>
       </c>
@@ -2239,18 +2383,20 @@
         <v>181</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B66" s="4"/>
+      <c r="B66" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C66" s="4" t="s">
         <v>182</v>
       </c>
@@ -2258,18 +2404,20 @@
         <v>183</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C67" s="4" t="s">
         <v>184</v>
       </c>
@@ -2277,7 +2425,7 @@
         <v>185</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>10</v>
@@ -2288,7 +2436,9 @@
       <c r="A68" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B68" s="4"/>
+      <c r="B68" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C68" s="4" t="s">
         <v>186</v>
       </c>
@@ -2296,18 +2446,20 @@
         <v>187</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B69" s="4"/>
+      <c r="B69" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C69" s="4" t="s">
         <v>188</v>
       </c>
@@ -2315,7 +2467,7 @@
         <v>189</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>10</v>
@@ -2326,7 +2478,9 @@
       <c r="A70" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C70" s="4" t="s">
         <v>190</v>
       </c>
@@ -2334,7 +2488,7 @@
         <v>191</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>10</v>
@@ -2345,7 +2499,9 @@
       <c r="A71" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C71" s="4" t="s">
         <v>192</v>
       </c>
@@ -2353,75 +2509,83 @@
         <v>193</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B72" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C72" s="4" t="s">
         <v>194</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="4"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G72" s="4"/>
-    </row>
-    <row r="73" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4" t="s">
+      <c r="D73" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>196</v>
+      <c r="E73" s="0" t="s">
+        <v>169</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B74" s="4"/>
+      <c r="B74" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C74" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="E74" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="F74" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B75" s="4"/>
+      <c r="B75" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C75" s="4" t="s">
         <v>201</v>
       </c>
@@ -2429,7 +2593,7 @@
         <v>202</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>13</v>
+        <v>200</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>10</v>
@@ -2437,25 +2601,33 @@
       <c r="G75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
+      <c r="A76" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C76" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D76" s="11" t="s">
+      <c r="D76" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E76" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C77" s="4" t="s">
         <v>205</v>
       </c>
@@ -2469,50 +2641,36 @@
         <v>10</v>
       </c>
       <c r="G77" s="4"/>
-      <c r="H77" s="4" t="s">
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="I77" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B78" s="4" t="s">
+      <c r="D78" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E78" s="4" t="s">
+      <c r="E78" s="11" t="s">
         <v>13</v>
       </c>
+      <c r="F78" s="4"/>
       <c r="G78" s="4"/>
-      <c r="H78" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="I78" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C79" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>13</v>
@@ -2521,22 +2679,25 @@
         <v>10</v>
       </c>
       <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
+      <c r="H79" s="4" t="s">
+        <v>211</v>
+      </c>
       <c r="I79" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B80" s="4"/>
+      <c r="B80" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C80" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D80" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>215</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>13</v>
@@ -2551,40 +2712,139 @@
       </c>
       <c r="J80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B81" s="4"/>
+      <c r="B81" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C81" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="I81" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J81" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="E81" s="4" t="s">
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J83" s="4"/>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F81" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-    </row>
+      <c r="F84" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C87" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="C34">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>#ref!=same</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="H78" r:id="rId1" display="https://www.academia.edu/1112558/Comparative_study_on_the_collection_of_data_to_measure_the_extent_and_impact_of_discrimination_within_the_United_States_Canada_Australia_the_United_Kingdom_and_the_Netherlands"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>